<commit_message>
a test table of strategies first edition up to true count 1
</commit_message>
<xml_diff>
--- a/test_table.xlsx
+++ b/test_table.xlsx
@@ -3123,16 +3123,56 @@
       <c r="G10" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="H10" s="7" t="n"/>
-      <c r="I10" s="7" t="n"/>
-      <c r="J10" s="7" t="n"/>
-      <c r="K10" s="7" t="n"/>
-      <c r="L10" s="7" t="n"/>
-      <c r="M10" s="7" t="n"/>
-      <c r="N10" s="7" t="n"/>
-      <c r="O10" s="7" t="n"/>
-      <c r="P10" s="7" t="n"/>
-      <c r="Q10" s="8" t="n"/>
+      <c r="H10" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="J10" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="K10" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="L10" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="M10" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="N10" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="O10" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="P10" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="Q10" s="8" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="18.75" customHeight="1">
       <c r="A11" s="9" t="n"/>
@@ -3144,16 +3184,56 @@
       <c r="G11" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="H11" s="7" t="n"/>
-      <c r="I11" s="7" t="n"/>
-      <c r="J11" s="7" t="n"/>
-      <c r="K11" s="7" t="n"/>
-      <c r="L11" s="7" t="n"/>
-      <c r="M11" s="7" t="n"/>
-      <c r="N11" s="7" t="n"/>
-      <c r="O11" s="7" t="n"/>
-      <c r="P11" s="7" t="n"/>
-      <c r="Q11" s="8" t="n"/>
+      <c r="H11" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="J11" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="K11" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="L11" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="M11" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N11" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O11" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P11" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="Q11" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="18.75" customHeight="1">
       <c r="A12" s="9" t="n"/>
@@ -3165,16 +3245,56 @@
       <c r="G12" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="H12" s="7" t="n"/>
-      <c r="I12" s="7" t="n"/>
-      <c r="J12" s="7" t="n"/>
-      <c r="K12" s="7" t="n"/>
-      <c r="L12" s="7" t="n"/>
-      <c r="M12" s="7" t="n"/>
-      <c r="N12" s="7" t="n"/>
-      <c r="O12" s="7" t="n"/>
-      <c r="P12" s="7" t="n"/>
-      <c r="Q12" s="8" t="n"/>
+      <c r="H12" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="I12" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="J12" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="K12" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="L12" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="M12" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N12" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O12" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P12" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q12" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="18.75" customHeight="1">
       <c r="A13" s="9" t="n"/>
@@ -3186,16 +3306,56 @@
       <c r="G13" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="H13" s="7" t="n"/>
-      <c r="I13" s="7" t="n"/>
-      <c r="J13" s="7" t="n"/>
-      <c r="K13" s="7" t="n"/>
-      <c r="L13" s="7" t="n"/>
-      <c r="M13" s="7" t="n"/>
-      <c r="N13" s="7" t="n"/>
-      <c r="O13" s="7" t="n"/>
-      <c r="P13" s="7" t="n"/>
-      <c r="Q13" s="8" t="n"/>
+      <c r="H13" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="I13" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="J13" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="K13" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="L13" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="M13" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N13" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O13" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P13" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q13" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="18.75" customHeight="1">
       <c r="A14" s="9" t="n"/>
@@ -3207,16 +3367,56 @@
       <c r="G14" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="H14" s="7" t="n"/>
-      <c r="I14" s="7" t="n"/>
-      <c r="J14" s="7" t="n"/>
-      <c r="K14" s="7" t="n"/>
-      <c r="L14" s="7" t="n"/>
-      <c r="M14" s="7" t="n"/>
-      <c r="N14" s="7" t="n"/>
-      <c r="O14" s="7" t="n"/>
-      <c r="P14" s="7" t="n"/>
-      <c r="Q14" s="8" t="n"/>
+      <c r="H14" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="I14" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="J14" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="K14" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="L14" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="M14" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N14" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O14" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P14" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q14" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="18.75" customHeight="1">
       <c r="A15" s="9" t="n"/>
@@ -3228,16 +3428,56 @@
       <c r="G15" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="H15" s="7" t="n"/>
-      <c r="I15" s="7" t="n"/>
-      <c r="J15" s="7" t="n"/>
-      <c r="K15" s="7" t="n"/>
-      <c r="L15" s="7" t="n"/>
-      <c r="M15" s="7" t="n"/>
-      <c r="N15" s="7" t="n"/>
-      <c r="O15" s="7" t="n"/>
-      <c r="P15" s="7" t="n"/>
-      <c r="Q15" s="8" t="n"/>
+      <c r="H15" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="I15" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="J15" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="K15" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="L15" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="M15" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N15" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O15" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P15" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q15" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="16" ht="18.75" customHeight="1">
       <c r="A16" s="9" t="n"/>
@@ -3249,16 +3489,56 @@
       <c r="G16" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="H16" s="7" t="n"/>
-      <c r="I16" s="7" t="n"/>
-      <c r="J16" s="7" t="n"/>
-      <c r="K16" s="7" t="n"/>
-      <c r="L16" s="7" t="n"/>
-      <c r="M16" s="7" t="n"/>
-      <c r="N16" s="7" t="n"/>
-      <c r="O16" s="7" t="n"/>
-      <c r="P16" s="7" t="n"/>
-      <c r="Q16" s="8" t="n"/>
+      <c r="H16" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="I16" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="J16" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="K16" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="L16" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="M16" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="N16" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="O16" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P16" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q16" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="17" ht="18.75" customHeight="1">
       <c r="A17" s="9" t="n"/>
@@ -3270,16 +3550,56 @@
       <c r="G17" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="H17" s="7" t="n"/>
-      <c r="I17" s="7" t="n"/>
-      <c r="J17" s="7" t="n"/>
-      <c r="K17" s="7" t="n"/>
-      <c r="L17" s="7" t="n"/>
-      <c r="M17" s="7" t="n"/>
-      <c r="N17" s="7" t="n"/>
-      <c r="O17" s="7" t="n"/>
-      <c r="P17" s="7" t="n"/>
-      <c r="Q17" s="8" t="n"/>
+      <c r="H17" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="I17" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="J17" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="K17" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="L17" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="M17" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="N17" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="O17" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P17" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q17" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="18" ht="18.75" customHeight="1">
       <c r="A18" s="9" t="n"/>
@@ -3291,16 +3611,56 @@
       <c r="G18" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="H18" s="7" t="n"/>
-      <c r="I18" s="7" t="n"/>
-      <c r="J18" s="7" t="n"/>
-      <c r="K18" s="7" t="n"/>
-      <c r="L18" s="7" t="n"/>
-      <c r="M18" s="7" t="n"/>
-      <c r="N18" s="7" t="n"/>
-      <c r="O18" s="7" t="n"/>
-      <c r="P18" s="7" t="n"/>
-      <c r="Q18" s="8" t="n"/>
+      <c r="H18" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="I18" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="J18" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="K18" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="L18" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="M18" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N18" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O18" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P18" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q18" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="19" ht="18.75" customHeight="1">
       <c r="A19" s="9" t="n"/>
@@ -3312,16 +3672,56 @@
       <c r="G19" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="H19" s="7" t="n"/>
-      <c r="I19" s="7" t="n"/>
-      <c r="J19" s="7" t="n"/>
-      <c r="K19" s="7" t="n"/>
-      <c r="L19" s="7" t="n"/>
-      <c r="M19" s="7" t="n"/>
-      <c r="N19" s="7" t="n"/>
-      <c r="O19" s="7" t="n"/>
-      <c r="P19" s="7" t="n"/>
-      <c r="Q19" s="8" t="n"/>
+      <c r="H19" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="I19" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="J19" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="K19" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="L19" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="M19" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N19" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O19" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P19" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q19" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="20" ht="18.75" customHeight="1">
       <c r="A20" s="9" t="n"/>
@@ -3333,16 +3733,56 @@
       <c r="G20" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="H20" s="7" t="n"/>
-      <c r="I20" s="7" t="n"/>
-      <c r="J20" s="7" t="n"/>
-      <c r="K20" s="7" t="n"/>
-      <c r="L20" s="7" t="n"/>
-      <c r="M20" s="7" t="n"/>
-      <c r="N20" s="7" t="n"/>
-      <c r="O20" s="7" t="n"/>
-      <c r="P20" s="7" t="n"/>
-      <c r="Q20" s="8" t="n"/>
+      <c r="H20" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="I20" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="J20" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="K20" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="L20" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="M20" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N20" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O20" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P20" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q20" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="21" ht="18.75" customHeight="1">
       <c r="A21" s="9" t="n"/>
@@ -3354,16 +3794,56 @@
       <c r="G21" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H21" s="7" t="n"/>
-      <c r="I21" s="7" t="n"/>
-      <c r="J21" s="7" t="n"/>
-      <c r="K21" s="7" t="n"/>
-      <c r="L21" s="7" t="n"/>
-      <c r="M21" s="7" t="n"/>
-      <c r="N21" s="7" t="n"/>
-      <c r="O21" s="7" t="n"/>
-      <c r="P21" s="7" t="n"/>
-      <c r="Q21" s="8" t="n"/>
+      <c r="H21" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="I21" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="J21" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="K21" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="L21" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="M21" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N21" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O21" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P21" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q21" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="22" ht="18.75" customHeight="1">
       <c r="A22" s="9" t="n"/>
@@ -3375,16 +3855,56 @@
       <c r="G22" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H22" s="7" t="n"/>
-      <c r="I22" s="7" t="n"/>
-      <c r="J22" s="7" t="n"/>
-      <c r="K22" s="7" t="n"/>
-      <c r="L22" s="7" t="n"/>
-      <c r="M22" s="7" t="n"/>
-      <c r="N22" s="7" t="n"/>
-      <c r="O22" s="7" t="n"/>
-      <c r="P22" s="7" t="n"/>
-      <c r="Q22" s="8" t="n"/>
+      <c r="H22" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="I22" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="J22" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="K22" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="L22" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="M22" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N22" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O22" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P22" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q22" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="23" ht="18.75" customHeight="1">
       <c r="A23" s="9" t="n"/>
@@ -3421,16 +3941,56 @@
           <t>A,9</t>
         </is>
       </c>
-      <c r="H24" s="7" t="n"/>
-      <c r="I24" s="7" t="n"/>
-      <c r="J24" s="7" t="n"/>
-      <c r="K24" s="7" t="n"/>
-      <c r="L24" s="7" t="n"/>
-      <c r="M24" s="7" t="n"/>
-      <c r="N24" s="7" t="n"/>
-      <c r="O24" s="7" t="n"/>
-      <c r="P24" s="7" t="n"/>
-      <c r="Q24" s="8" t="n"/>
+      <c r="H24" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="I24" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="J24" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="K24" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="L24" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="M24" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="N24" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="O24" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="P24" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="Q24" s="8" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="25" ht="18.75" customHeight="1">
       <c r="A25" s="9" t="n"/>
@@ -3444,16 +4004,56 @@
           <t>A,8</t>
         </is>
       </c>
-      <c r="H25" s="7" t="n"/>
-      <c r="I25" s="7" t="n"/>
-      <c r="J25" s="7" t="n"/>
-      <c r="K25" s="7" t="n"/>
-      <c r="L25" s="7" t="n"/>
-      <c r="M25" s="7" t="n"/>
-      <c r="N25" s="7" t="n"/>
-      <c r="O25" s="7" t="n"/>
-      <c r="P25" s="7" t="n"/>
-      <c r="Q25" s="8" t="n"/>
+      <c r="H25" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="I25" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="J25" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="K25" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="L25" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="M25" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="N25" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="O25" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="P25" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="Q25" s="8" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="26" ht="18.75" customHeight="1">
       <c r="A26" s="9" t="n"/>
@@ -3467,16 +4067,56 @@
           <t>A,7</t>
         </is>
       </c>
-      <c r="H26" s="7" t="n"/>
-      <c r="I26" s="7" t="n"/>
-      <c r="J26" s="7" t="n"/>
-      <c r="K26" s="7" t="n"/>
-      <c r="L26" s="7" t="n"/>
-      <c r="M26" s="7" t="n"/>
-      <c r="N26" s="7" t="n"/>
-      <c r="O26" s="7" t="n"/>
-      <c r="P26" s="7" t="n"/>
-      <c r="Q26" s="8" t="n"/>
+      <c r="H26" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="I26" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="J26" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="K26" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="L26" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="M26" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="N26" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="O26" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P26" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q26" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="27" ht="18.75" customHeight="1">
       <c r="A27" s="9" t="n"/>
@@ -3490,16 +4130,56 @@
           <t>A,6</t>
         </is>
       </c>
-      <c r="H27" s="7" t="n"/>
-      <c r="I27" s="7" t="n"/>
-      <c r="J27" s="7" t="n"/>
-      <c r="K27" s="7" t="n"/>
-      <c r="L27" s="7" t="n"/>
-      <c r="M27" s="7" t="n"/>
-      <c r="N27" s="7" t="n"/>
-      <c r="O27" s="7" t="n"/>
-      <c r="P27" s="7" t="n"/>
-      <c r="Q27" s="8" t="n"/>
+      <c r="H27" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="I27" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="J27" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="K27" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="L27" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="M27" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N27" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O27" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P27" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q27" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="28" ht="18.75" customHeight="1">
       <c r="A28" s="9" t="n"/>
@@ -3513,16 +4193,56 @@
           <t>A,5</t>
         </is>
       </c>
-      <c r="H28" s="7" t="n"/>
-      <c r="I28" s="7" t="n"/>
-      <c r="J28" s="7" t="n"/>
-      <c r="K28" s="7" t="n"/>
-      <c r="L28" s="7" t="n"/>
-      <c r="M28" s="7" t="n"/>
-      <c r="N28" s="7" t="n"/>
-      <c r="O28" s="7" t="n"/>
-      <c r="P28" s="7" t="n"/>
-      <c r="Q28" s="8" t="n"/>
+      <c r="H28" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="I28" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="J28" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="K28" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="L28" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="M28" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N28" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O28" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P28" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q28" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="29" ht="18.75" customHeight="1">
       <c r="A29" s="9" t="n"/>
@@ -3536,16 +4256,56 @@
           <t>A,4</t>
         </is>
       </c>
-      <c r="H29" s="7" t="n"/>
-      <c r="I29" s="7" t="n"/>
-      <c r="J29" s="7" t="n"/>
-      <c r="K29" s="7" t="n"/>
-      <c r="L29" s="7" t="n"/>
-      <c r="M29" s="7" t="n"/>
-      <c r="N29" s="7" t="n"/>
-      <c r="O29" s="7" t="n"/>
-      <c r="P29" s="7" t="n"/>
-      <c r="Q29" s="8" t="n"/>
+      <c r="H29" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="I29" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="J29" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="K29" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="L29" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="M29" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N29" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O29" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P29" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q29" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="30" ht="18.75" customHeight="1">
       <c r="A30" s="9" t="n"/>
@@ -3559,16 +4319,56 @@
           <t>A,3</t>
         </is>
       </c>
-      <c r="H30" s="7" t="n"/>
-      <c r="I30" s="7" t="n"/>
-      <c r="J30" s="7" t="n"/>
-      <c r="K30" s="7" t="n"/>
-      <c r="L30" s="7" t="n"/>
-      <c r="M30" s="7" t="n"/>
-      <c r="N30" s="7" t="n"/>
-      <c r="O30" s="7" t="n"/>
-      <c r="P30" s="7" t="n"/>
-      <c r="Q30" s="8" t="n"/>
+      <c r="H30" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="I30" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="J30" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="K30" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="L30" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="M30" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N30" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O30" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P30" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q30" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="31" ht="18.75" customHeight="1">
       <c r="A31" s="9" t="n"/>
@@ -3582,16 +4382,56 @@
           <t>A,2</t>
         </is>
       </c>
-      <c r="H31" s="7" t="n"/>
-      <c r="I31" s="7" t="n"/>
-      <c r="J31" s="7" t="n"/>
-      <c r="K31" s="7" t="n"/>
-      <c r="L31" s="7" t="n"/>
-      <c r="M31" s="7" t="n"/>
-      <c r="N31" s="7" t="n"/>
-      <c r="O31" s="7" t="n"/>
-      <c r="P31" s="7" t="n"/>
-      <c r="Q31" s="8" t="n"/>
+      <c r="H31" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="I31" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="J31" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="K31" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="L31" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="M31" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N31" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O31" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P31" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q31" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="32" ht="18.75" customHeight="1">
       <c r="A32" s="9" t="n"/>
@@ -3628,16 +4468,56 @@
           <t>10,10</t>
         </is>
       </c>
-      <c r="H33" s="7" t="n"/>
-      <c r="I33" s="7" t="n"/>
-      <c r="J33" s="7" t="n"/>
-      <c r="K33" s="7" t="n"/>
-      <c r="L33" s="7" t="n"/>
-      <c r="M33" s="7" t="n"/>
-      <c r="N33" s="7" t="n"/>
-      <c r="O33" s="7" t="n"/>
-      <c r="P33" s="7" t="n"/>
-      <c r="Q33" s="8" t="n"/>
+      <c r="H33" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="I33" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="J33" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="K33" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="L33" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="M33" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="N33" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="O33" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="P33" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="Q33" s="8" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="34" ht="18.75" customHeight="1">
       <c r="A34" s="9" t="n"/>
@@ -3651,16 +4531,56 @@
           <t>9,9</t>
         </is>
       </c>
-      <c r="H34" s="7" t="n"/>
-      <c r="I34" s="7" t="n"/>
-      <c r="J34" s="7" t="n"/>
-      <c r="K34" s="7" t="n"/>
-      <c r="L34" s="7" t="n"/>
-      <c r="M34" s="7" t="n"/>
-      <c r="N34" s="7" t="n"/>
-      <c r="O34" s="7" t="n"/>
-      <c r="P34" s="7" t="n"/>
-      <c r="Q34" s="8" t="n"/>
+      <c r="H34" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="I34" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="J34" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="K34" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="L34" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="M34" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="N34" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="O34" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="P34" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="Q34" s="8" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="35" ht="18.75" customHeight="1">
       <c r="A35" s="9" t="n"/>
@@ -3674,16 +4594,56 @@
           <t>8,8</t>
         </is>
       </c>
-      <c r="H35" s="7" t="n"/>
-      <c r="I35" s="7" t="n"/>
-      <c r="J35" s="7" t="n"/>
-      <c r="K35" s="7" t="n"/>
-      <c r="L35" s="7" t="n"/>
-      <c r="M35" s="7" t="n"/>
-      <c r="N35" s="7" t="n"/>
-      <c r="O35" s="7" t="n"/>
-      <c r="P35" s="7" t="n"/>
-      <c r="Q35" s="8" t="n"/>
+      <c r="H35" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="I35" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="J35" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="K35" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="L35" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="M35" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="N35" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="O35" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="P35" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="Q35" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="36" ht="18.75" customHeight="1">
       <c r="A36" s="9" t="n"/>
@@ -3697,16 +4657,56 @@
           <t>7,7</t>
         </is>
       </c>
-      <c r="H36" s="7" t="n"/>
-      <c r="I36" s="7" t="n"/>
-      <c r="J36" s="7" t="n"/>
-      <c r="K36" s="7" t="n"/>
-      <c r="L36" s="7" t="n"/>
-      <c r="M36" s="7" t="n"/>
-      <c r="N36" s="7" t="n"/>
-      <c r="O36" s="7" t="n"/>
-      <c r="P36" s="7" t="n"/>
-      <c r="Q36" s="8" t="n"/>
+      <c r="H36" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="I36" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="J36" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="K36" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="L36" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="M36" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="N36" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O36" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P36" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q36" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="37" ht="18.75" customHeight="1">
       <c r="A37" s="9" t="n"/>
@@ -3720,16 +4720,56 @@
           <t>6,6</t>
         </is>
       </c>
-      <c r="H37" s="7" t="n"/>
-      <c r="I37" s="7" t="n"/>
-      <c r="J37" s="7" t="n"/>
-      <c r="K37" s="7" t="n"/>
-      <c r="L37" s="7" t="n"/>
-      <c r="M37" s="7" t="n"/>
-      <c r="N37" s="7" t="n"/>
-      <c r="O37" s="7" t="n"/>
-      <c r="P37" s="7" t="n"/>
-      <c r="Q37" s="8" t="n"/>
+      <c r="H37" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="I37" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="J37" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="K37" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="L37" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="M37" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N37" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O37" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P37" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q37" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="38" ht="18.75" customHeight="1">
       <c r="A38" s="9" t="n"/>
@@ -3743,16 +4783,56 @@
           <t>5,5</t>
         </is>
       </c>
-      <c r="H38" s="7" t="n"/>
-      <c r="I38" s="7" t="n"/>
-      <c r="J38" s="7" t="n"/>
-      <c r="K38" s="7" t="n"/>
-      <c r="L38" s="7" t="n"/>
-      <c r="M38" s="7" t="n"/>
-      <c r="N38" s="7" t="n"/>
-      <c r="O38" s="7" t="n"/>
-      <c r="P38" s="7" t="n"/>
-      <c r="Q38" s="8" t="n"/>
+      <c r="H38" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="I38" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="J38" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="K38" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="L38" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="M38" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="N38" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O38" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P38" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q38" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="39" ht="18.75" customHeight="1">
       <c r="A39" s="9" t="n"/>
@@ -3766,16 +4846,56 @@
           <t>4,4</t>
         </is>
       </c>
-      <c r="H39" s="7" t="n"/>
-      <c r="I39" s="7" t="n"/>
-      <c r="J39" s="7" t="n"/>
-      <c r="K39" s="7" t="n"/>
-      <c r="L39" s="7" t="n"/>
-      <c r="M39" s="7" t="n"/>
-      <c r="N39" s="7" t="n"/>
-      <c r="O39" s="7" t="n"/>
-      <c r="P39" s="7" t="n"/>
-      <c r="Q39" s="8" t="n"/>
+      <c r="H39" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="I39" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="J39" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="K39" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="L39" s="7" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="M39" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N39" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O39" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P39" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q39" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="40" ht="18.75" customHeight="1">
       <c r="A40" s="9" t="n"/>
@@ -3789,16 +4909,56 @@
           <t>3,3</t>
         </is>
       </c>
-      <c r="H40" s="7" t="n"/>
-      <c r="I40" s="7" t="n"/>
-      <c r="J40" s="7" t="n"/>
-      <c r="K40" s="7" t="n"/>
-      <c r="L40" s="7" t="n"/>
-      <c r="M40" s="7" t="n"/>
-      <c r="N40" s="7" t="n"/>
-      <c r="O40" s="7" t="n"/>
-      <c r="P40" s="7" t="n"/>
-      <c r="Q40" s="8" t="n"/>
+      <c r="H40" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="I40" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="J40" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="K40" s="7" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="L40" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="M40" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N40" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O40" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P40" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q40" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="41" ht="18.75" customHeight="1">
       <c r="A41" s="9" t="n"/>
@@ -3812,16 +4972,56 @@
           <t>2,2</t>
         </is>
       </c>
-      <c r="H41" s="7" t="n"/>
-      <c r="I41" s="7" t="n"/>
-      <c r="J41" s="7" t="n"/>
-      <c r="K41" s="7" t="n"/>
-      <c r="L41" s="7" t="n"/>
-      <c r="M41" s="7" t="n"/>
-      <c r="N41" s="7" t="n"/>
-      <c r="O41" s="7" t="n"/>
-      <c r="P41" s="7" t="n"/>
-      <c r="Q41" s="8" t="n"/>
+      <c r="H41" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="I41" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="J41" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="K41" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="L41" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="M41" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="N41" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="O41" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P41" s="7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="Q41" s="8" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>